<commit_message>
new results from message-level
</commit_message>
<xml_diff>
--- a/classification/droptc/message/bert-base-uncased/freeze/14298463/prediction.xlsx
+++ b/classification/droptc/message/bert-base-uncased/freeze/14298463/prediction.xlsx
@@ -1531,12 +1531,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0, 0, 0, 0]</t>
+          <t>[1, 0, 1, 0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>['Normal']</t>
+          <t>['Normal', 'HardwareFault']</t>
         </is>
       </c>
     </row>

</xml_diff>